<commit_message>
all error msg has been handeled
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zapta\Automation\Lahebo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76871B39-E01D-43D9-AEDE-9B7653F01295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7507C40-CDB9-4FCD-B744-30A46B6D4B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="168">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -185,15 +185,6 @@
     <t>explorer33@packiu.com</t>
   </si>
   <si>
-    <t>explorer33</t>
-  </si>
-  <si>
-    <t>Zubair</t>
-  </si>
-  <si>
-    <t>Amin</t>
-  </si>
-  <si>
     <t>ubelibervalent1990w</t>
   </si>
   <si>
@@ -252,13 +243,301 @@
   </si>
   <si>
     <t>login Pass with correct username and correct password</t>
+  </si>
+  <si>
+    <t>johnpaul33</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>jane.doe@example.com</t>
+  </si>
+  <si>
+    <t>janedoe123</t>
+  </si>
+  <si>
+    <t>Pa$$w0rd</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>acme</t>
+  </si>
+  <si>
+    <t>michael.smith@gmail.com</t>
+  </si>
+  <si>
+    <t>msmith123</t>
+  </si>
+  <si>
+    <t>StrongP@ssword1</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>sarahj@example.com</t>
+  </si>
+  <si>
+    <t>sarahj88</t>
+  </si>
+  <si>
+    <t>Password123!</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>j.brown@example.com</t>
+  </si>
+  <si>
+    <t>jbrown12</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>adam@example.com</t>
+  </si>
+  <si>
+    <t>adam123</t>
+  </si>
+  <si>
+    <t>P@ssw0rd!</t>
+  </si>
+  <si>
+    <t>Valid test case, all fields have valid values</t>
+  </si>
+  <si>
+    <t>Invalid phone number (not an Australian mobile number)</t>
+  </si>
+  <si>
+    <t>Empty field (ORGANISATION_NAME)</t>
+  </si>
+  <si>
+    <t>Empty field (LAST_NAME)</t>
+  </si>
+  <si>
+    <t>Empty fields (FIRST_NAME, LAST_NAME, EMAIL, USERNAME)</t>
+  </si>
+  <si>
+    <t>Invalid password (less than 8 characters)</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>alex@example.com</t>
+  </si>
+  <si>
+    <t>alexand123</t>
+  </si>
+  <si>
+    <t>Short1!</t>
+  </si>
+  <si>
+    <t>Invalid phone number (less than 10 digits)</t>
+  </si>
+  <si>
+    <t>john@acme.com</t>
+  </si>
+  <si>
+    <t>john_smith</t>
+  </si>
+  <si>
+    <t>Invalid password (does not meet complexity requirements)</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>karen@example.com</t>
+  </si>
+  <si>
+    <t>karenw123</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Empty field (FIRST_NAME)</t>
+  </si>
+  <si>
+    <t>Invalid email format</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>mark.johnson</t>
+  </si>
+  <si>
+    <t>markj123</t>
+  </si>
+  <si>
+    <t>Invalid password (missing uppercase letter)</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>jennifer@example.com</t>
+  </si>
+  <si>
+    <t>jensmith</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>Invalid password (missing lowercase letter)</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>TESTCASE_SCENARIO</t>
+  </si>
+  <si>
+    <t>alex.green@example.com</t>
+  </si>
+  <si>
+    <t>alexgreen</t>
+  </si>
+  <si>
+    <t>PASSWORD1</t>
+  </si>
+  <si>
+    <t>Invalid password (missing number)</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>sarah.taylor@example.com</t>
+  </si>
+  <si>
+    <t>saraht123</t>
+  </si>
+  <si>
+    <t>Passw0rd!</t>
+  </si>
+  <si>
+    <t>Invalid password (missing special character)</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>john.parker@example.com</t>
+  </si>
+  <si>
+    <t>johnparker</t>
+  </si>
+  <si>
+    <t>Pssw0rd</t>
+  </si>
+  <si>
+    <t>Invalid password (mismatch between password and confirm password)</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>robert.wilson@example.com</t>
+  </si>
+  <si>
+    <t>robertw123</t>
+  </si>
+  <si>
+    <t>Password456!</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t>TC017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,12 +644,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF777777"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -379,7 +652,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,11 +663,6 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
       </patternFill>
     </fill>
   </fills>
@@ -411,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -442,20 +710,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -775,7 +1037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -785,7 +1047,7 @@
     <col min="2" max="2" width="75.28515625" style="10" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="32.85546875" style="10" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="38" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="20.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17.28515625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="22.85546875" style="10" customWidth="1" collapsed="1"/>
@@ -795,7 +1057,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>11</v>
@@ -816,22 +1078,22 @@
         <v>27</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="A2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>56</v>
+      <c r="E2" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -839,18 +1101,18 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="A3" s="14" t="s">
         <v>56</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -858,83 +1120,83 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="18" t="s">
+      <c r="C7" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="18" t="s">
+      <c r="C8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -942,35 +1204,35 @@
       <c r="B9" s="11"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9" s="16"/>
+      <c r="E9" s="12"/>
       <c r="F9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
       <c r="C10"/>
       <c r="D10"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="12"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
       <c r="C11"/>
       <c r="D11"/>
-      <c r="E11" s="16"/>
+      <c r="E11" s="12"/>
       <c r="F11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
       <c r="C12"/>
       <c r="D12"/>
-      <c r="E12" s="16"/>
+      <c r="E12" s="12"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="11"/>
       <c r="C13"/>
       <c r="D13"/>
-      <c r="E13" s="16"/>
+      <c r="E13" s="12"/>
       <c r="F13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1000,147 +1262,635 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="15">
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2">
         <v>3197010517646</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3">
+        <v>401123456</v>
+      </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4">
+        <v>412345678</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5">
+        <v>456789012</v>
+      </c>
+      <c r="K5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="15">
-        <v>3197010517646</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8">
+        <v>467890123</v>
+      </c>
+      <c r="I8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9">
+        <v>412</v>
+      </c>
+      <c r="I9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" t="s">
+        <v>80</v>
+      </c>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10">
+        <v>1234567890</v>
+      </c>
+      <c r="I10" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11">
+        <v>467890123</v>
+      </c>
+      <c r="I11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12">
+        <v>434567890</v>
+      </c>
+      <c r="I12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" t="s">
+        <v>98</v>
+      </c>
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13">
+        <v>478901234</v>
+      </c>
+      <c r="I13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" t="s">
+        <v>128</v>
+      </c>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14">
+        <v>412345678</v>
+      </c>
+      <c r="I14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" t="s">
+        <v>134</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15">
+        <v>423456789</v>
+      </c>
+      <c r="I15" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" t="s">
+        <v>139</v>
+      </c>
+      <c r="K15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16">
+        <v>434567890</v>
+      </c>
+      <c r="I16" t="s">
+        <v>144</v>
+      </c>
+      <c r="J16" t="s">
+        <v>144</v>
+      </c>
+      <c r="K16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17">
+        <v>456789012</v>
+      </c>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" t="s">
+        <v>150</v>
+      </c>
+      <c r="K17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18">
+        <v>423456789</v>
+      </c>
+      <c r="I18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="mailto:explorer33@packiu.com" xr:uid="{BDFC285A-DDFB-4738-A77A-60F692EB6A41}"/>
+    <hyperlink ref="F3" r:id="rId2" display="mailto:jane.doe@example.com" xr:uid="{67032504-2918-45EE-BA50-8C04BED9D910}"/>
+    <hyperlink ref="F4" r:id="rId3" display="mailto:michael.smith@gmail.com" xr:uid="{E556A35B-1BBA-4B19-A0CA-F6385D9E9581}"/>
+    <hyperlink ref="F5" r:id="rId4" display="mailto:j.brown@example.com" xr:uid="{9DFE164D-E2A8-4667-9D6B-8F61C02A77AF}"/>
+    <hyperlink ref="F6" r:id="rId5" display="mailto:adam@example.com" xr:uid="{6A4AF44C-6C03-4BD4-B4D2-F2A8A366E654}"/>
+    <hyperlink ref="F8" r:id="rId6" display="mailto:alex@example.com" xr:uid="{F0483DD7-F3D2-461E-B495-C03875C8D962}"/>
+    <hyperlink ref="F9" r:id="rId7" display="mailto:john@acme.com" xr:uid="{8721B45D-11B3-4BFD-AFC8-EBEEAEACDA5D}"/>
+    <hyperlink ref="F10" r:id="rId8" display="mailto:karen@example.com" xr:uid="{0ACC85B6-6103-4AF5-9E36-6AD2972C63AB}"/>
+    <hyperlink ref="F11" r:id="rId9" display="mailto:alex@example.com" xr:uid="{1FCC9A60-CF5F-4058-9BF2-182F9145EA22}"/>
+    <hyperlink ref="F13" r:id="rId10" display="mailto:jennifer@example.com" xr:uid="{F51E6647-6FC6-40FB-BA5C-FC1428669E58}"/>
+    <hyperlink ref="F14" r:id="rId11" display="mailto:alex.green@example.com" xr:uid="{9EDBBE42-7C14-4EA9-A701-5E09B00666AE}"/>
+    <hyperlink ref="F15" r:id="rId12" display="mailto:sarah.taylor@example.com" xr:uid="{5CFDE6E9-D087-4E1D-8BA1-24C52B201C38}"/>
+    <hyperlink ref="F16" r:id="rId13" display="mailto:john.parker@example.com" xr:uid="{C8F5619E-E92F-4E79-A833-38F9B4BEEF58}"/>
+    <hyperlink ref="F17" r:id="rId14" display="mailto:robert.wilson@example.com" xr:uid="{75FE90AA-72BB-4B81-A820-12FEC320BF5A}"/>
+    <hyperlink ref="F18" r:id="rId15" display="mailto:sarahj@example.com" xr:uid="{F06DEF8D-DB30-4097-B986-F23CC9BFA85C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sign up completed just need minor finishing
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zapta\Automation\Lahebo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7507C40-CDB9-4FCD-B744-30A46B6D4B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0F8E98-4933-481D-9640-CB0C27AC01B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
     <sheet name="SignUp" sheetId="4" r:id="rId2"/>
-    <sheet name="Client" sheetId="1" r:id="rId3"/>
+    <sheet name="NewUser" sheetId="5" r:id="rId3"/>
+    <sheet name="Client" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -296,9 +297,6 @@
     <t>Johnson</t>
   </si>
   <si>
-    <t>sarahj@example.com</t>
-  </si>
-  <si>
     <t>sarahj88</t>
   </si>
   <si>
@@ -531,13 +529,16 @@
   </si>
   <si>
     <t>TC017</t>
+  </si>
+  <si>
+    <t>zubairulamin8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,6 +652,11 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444746"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -679,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -720,6 +726,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1265,7 +1272,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1293,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>44</v>
@@ -1324,10 +1331,10 @@
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
@@ -1361,10 +1368,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>74</v>
@@ -1396,10 +1403,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>81</v>
@@ -1431,22 +1438,22 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
         <v>76</v>
       </c>
       <c r="F5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" t="s">
         <v>93</v>
-      </c>
-      <c r="G5" t="s">
-        <v>94</v>
       </c>
       <c r="H5">
         <v>456789012</v>
@@ -1457,28 +1464,28 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
       <c r="F6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" t="s">
         <v>96</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>97</v>
       </c>
-      <c r="I6" t="s">
-        <v>98</v>
-      </c>
       <c r="J6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K6" t="s">
         <v>80</v>
@@ -1486,10 +1493,10 @@
     </row>
     <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K7" t="s">
         <v>80</v>
@@ -1499,31 +1506,31 @@
     </row>
     <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
         <v>104</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>105</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>106</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>107</v>
-      </c>
-      <c r="G8" t="s">
-        <v>108</v>
       </c>
       <c r="H8">
         <v>467890123</v>
       </c>
       <c r="I8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K8" t="s">
         <v>80</v>
@@ -1533,28 +1540,28 @@
     </row>
     <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
         <v>83</v>
       </c>
       <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="s">
         <v>111</v>
-      </c>
-      <c r="G9" t="s">
-        <v>112</v>
       </c>
       <c r="H9">
         <v>412</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K9" t="s">
         <v>80</v>
@@ -1564,34 +1571,34 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="s">
         <v>113</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>114</v>
-      </c>
-      <c r="D10" t="s">
-        <v>115</v>
       </c>
       <c r="E10" t="s">
         <v>76</v>
       </c>
       <c r="F10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" t="s">
         <v>116</v>
-      </c>
-      <c r="G10" t="s">
-        <v>117</v>
       </c>
       <c r="H10">
         <v>1234567890</v>
       </c>
       <c r="I10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K10" t="s">
         <v>80</v>
@@ -1599,28 +1606,28 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" t="s">
         <v>106</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>107</v>
-      </c>
-      <c r="G11" t="s">
-        <v>108</v>
       </c>
       <c r="H11">
         <v>467890123</v>
       </c>
       <c r="I11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K11" t="s">
         <v>80</v>
@@ -1628,13 +1635,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
         <v>120</v>
-      </c>
-      <c r="C12" t="s">
-        <v>121</v>
       </c>
       <c r="D12" t="s">
         <v>88</v>
@@ -1643,19 +1650,19 @@
         <v>50</v>
       </c>
       <c r="F12" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" t="s">
         <v>122</v>
-      </c>
-      <c r="G12" t="s">
-        <v>123</v>
       </c>
       <c r="H12">
         <v>434567890</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K12" t="s">
         <v>80</v>
@@ -1663,13 +1670,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
         <v>124</v>
-      </c>
-      <c r="C13" t="s">
-        <v>125</v>
       </c>
       <c r="D13" t="s">
         <v>82</v>
@@ -1678,19 +1685,19 @@
         <v>76</v>
       </c>
       <c r="F13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" t="s">
         <v>126</v>
-      </c>
-      <c r="G13" t="s">
-        <v>127</v>
       </c>
       <c r="H13">
         <v>478901234</v>
       </c>
       <c r="I13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K13" t="s">
         <v>80</v>
@@ -1698,34 +1705,34 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
         <v>129</v>
-      </c>
-      <c r="C14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D14" t="s">
-        <v>130</v>
       </c>
       <c r="E14" t="s">
         <v>83</v>
       </c>
       <c r="F14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" t="s">
         <v>132</v>
-      </c>
-      <c r="G14" t="s">
-        <v>133</v>
       </c>
       <c r="H14">
         <v>412345678</v>
       </c>
       <c r="I14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K14" t="s">
         <v>80</v>
@@ -1733,34 +1740,34 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
         <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
         <v>50</v>
       </c>
       <c r="F15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" t="s">
         <v>137</v>
-      </c>
-      <c r="G15" t="s">
-        <v>138</v>
       </c>
       <c r="H15">
         <v>423456789</v>
       </c>
       <c r="I15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K15" t="s">
         <v>80</v>
@@ -1768,34 +1775,34 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" t="s">
         <v>76</v>
       </c>
       <c r="F16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" t="s">
         <v>142</v>
-      </c>
-      <c r="G16" t="s">
-        <v>143</v>
       </c>
       <c r="H16">
         <v>434567890</v>
       </c>
       <c r="I16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K16" t="s">
         <v>80</v>
@@ -1803,34 +1810,34 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" t="s">
         <v>145</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>146</v>
-      </c>
-      <c r="D17" t="s">
-        <v>147</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
       </c>
       <c r="F17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" t="s">
         <v>148</v>
-      </c>
-      <c r="G17" t="s">
-        <v>149</v>
       </c>
       <c r="H17">
         <v>456789012</v>
       </c>
       <c r="I17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K17" t="s">
         <v>80</v>
@@ -1838,10 +1845,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
         <v>87</v>
@@ -1852,20 +1859,20 @@
       <c r="E18" t="s">
         <v>50</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" t="s">
         <v>89</v>
-      </c>
-      <c r="G18" t="s">
-        <v>90</v>
       </c>
       <c r="H18">
         <v>423456789</v>
       </c>
       <c r="I18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K18" t="s">
         <v>73</v>
@@ -1887,19 +1894,32 @@
     <hyperlink ref="F15" r:id="rId12" display="mailto:sarah.taylor@example.com" xr:uid="{5CFDE6E9-D087-4E1D-8BA1-24C52B201C38}"/>
     <hyperlink ref="F16" r:id="rId13" display="mailto:john.parker@example.com" xr:uid="{C8F5619E-E92F-4E79-A833-38F9B4BEEF58}"/>
     <hyperlink ref="F17" r:id="rId14" display="mailto:robert.wilson@example.com" xr:uid="{75FE90AA-72BB-4B81-A820-12FEC320BF5A}"/>
-    <hyperlink ref="F18" r:id="rId15" display="mailto:sarahj@example.com" xr:uid="{F06DEF8D-DB30-4097-B986-F23CC9BFA85C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE0024C-58FB-4382-99F9-AF515DDACB52}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
signup completed with saving new user credentials into config file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zapta\Automation\Lahebo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0F8E98-4933-481D-9640-CB0C27AC01B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A579794D-4190-4B4C-BD1F-C584AE09D2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="170">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -183,9 +183,6 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>explorer33@packiu.com</t>
-  </si>
-  <si>
     <t>ubelibervalent1990w</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>abc</t>
   </si>
   <si>
-    <t>jane.doe@example.com</t>
-  </si>
-  <si>
     <t>janedoe123</t>
   </si>
   <si>
@@ -282,9 +276,6 @@
     <t>acme</t>
   </si>
   <si>
-    <t>michael.smith@gmail.com</t>
-  </si>
-  <si>
     <t>msmith123</t>
   </si>
   <si>
@@ -306,9 +297,6 @@
     <t>Brown</t>
   </si>
   <si>
-    <t>j.brown@example.com</t>
-  </si>
-  <si>
     <t>jbrown12</t>
   </si>
   <si>
@@ -360,9 +348,6 @@
     <t>Invalid phone number (less than 10 digits)</t>
   </si>
   <si>
-    <t>john@acme.com</t>
-  </si>
-  <si>
     <t>john_smith</t>
   </si>
   <si>
@@ -375,9 +360,6 @@
     <t>Williams</t>
   </si>
   <si>
-    <t>karen@example.com</t>
-  </si>
-  <si>
     <t>karenw123</t>
   </si>
   <si>
@@ -532,6 +514,30 @@
   </si>
   <si>
     <t>zubairulamin8</t>
+  </si>
+  <si>
+    <t>explorer353@packiu.com</t>
+  </si>
+  <si>
+    <t>jane.d2oe@example.com</t>
+  </si>
+  <si>
+    <t>michael.sm3ith@gmail.com</t>
+  </si>
+  <si>
+    <t>j.brow3n@example.com</t>
+  </si>
+  <si>
+    <t>StrongP2ssword1</t>
+  </si>
+  <si>
+    <t>ale3x@example.com</t>
+  </si>
+  <si>
+    <t>joh5n@acme.com</t>
+  </si>
+  <si>
+    <t>kar8en@example.com</t>
   </si>
 </sst>
 </file>
@@ -685,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -727,6 +733,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1064,7 +1071,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>11</v>
@@ -1085,22 +1092,22 @@
         <v>27</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -1109,17 +1116,17 @@
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -1128,23 +1135,23 @@
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>36</v>
@@ -1153,52 +1160,52 @@
         <v>35</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>43</v>
@@ -1272,7 +1279,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1300,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>44</v>
@@ -1331,10 +1338,10 @@
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
@@ -1346,10 +1353,10 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2">
         <v>3197010517646</v>
@@ -1361,542 +1368,543 @@
         <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>75</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" t="s">
         <v>76</v>
-      </c>
-      <c r="F3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" t="s">
-        <v>78</v>
       </c>
       <c r="H3">
         <v>401123456</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
         <v>81</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" t="s">
         <v>82</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
       </c>
       <c r="H4">
         <v>412345678</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" t="s">
-        <v>92</v>
+        <v>75</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H5">
         <v>456789012</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" t="s">
         <v>103</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" t="s">
-        <v>107</v>
       </c>
       <c r="H8">
         <v>467890123</v>
       </c>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" t="s">
-        <v>110</v>
+        <v>81</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="G9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H9">
         <v>412</v>
       </c>
       <c r="I9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" t="s">
-        <v>115</v>
+        <v>75</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H10">
         <v>1234567890</v>
       </c>
       <c r="I10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="J10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H11">
         <v>467890123</v>
       </c>
       <c r="I11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
         <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H12">
         <v>434567890</v>
       </c>
       <c r="I12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H13">
         <v>478901234</v>
       </c>
       <c r="I13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="J13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="K13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G14" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H14">
         <v>412345678</v>
       </c>
       <c r="I14" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J14" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E15" t="s">
         <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G15" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H15">
         <v>423456789</v>
       </c>
       <c r="I15" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J15" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G16" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H16">
         <v>434567890</v>
       </c>
       <c r="I16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G17" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H17">
         <v>456789012</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E18" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H18">
         <v>423456789</v>
       </c>
       <c r="I18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="mailto:explorer33@packiu.com" xr:uid="{BDFC285A-DDFB-4738-A77A-60F692EB6A41}"/>
-    <hyperlink ref="F3" r:id="rId2" display="mailto:jane.doe@example.com" xr:uid="{67032504-2918-45EE-BA50-8C04BED9D910}"/>
-    <hyperlink ref="F4" r:id="rId3" display="mailto:michael.smith@gmail.com" xr:uid="{E556A35B-1BBA-4B19-A0CA-F6385D9E9581}"/>
-    <hyperlink ref="F5" r:id="rId4" display="mailto:j.brown@example.com" xr:uid="{9DFE164D-E2A8-4667-9D6B-8F61C02A77AF}"/>
-    <hyperlink ref="F6" r:id="rId5" display="mailto:adam@example.com" xr:uid="{6A4AF44C-6C03-4BD4-B4D2-F2A8A366E654}"/>
-    <hyperlink ref="F8" r:id="rId6" display="mailto:alex@example.com" xr:uid="{F0483DD7-F3D2-461E-B495-C03875C8D962}"/>
-    <hyperlink ref="F9" r:id="rId7" display="mailto:john@acme.com" xr:uid="{8721B45D-11B3-4BFD-AFC8-EBEEAEACDA5D}"/>
-    <hyperlink ref="F10" r:id="rId8" display="mailto:karen@example.com" xr:uid="{0ACC85B6-6103-4AF5-9E36-6AD2972C63AB}"/>
-    <hyperlink ref="F11" r:id="rId9" display="mailto:alex@example.com" xr:uid="{1FCC9A60-CF5F-4058-9BF2-182F9145EA22}"/>
-    <hyperlink ref="F13" r:id="rId10" display="mailto:jennifer@example.com" xr:uid="{F51E6647-6FC6-40FB-BA5C-FC1428669E58}"/>
-    <hyperlink ref="F14" r:id="rId11" display="mailto:alex.green@example.com" xr:uid="{9EDBBE42-7C14-4EA9-A701-5E09B00666AE}"/>
-    <hyperlink ref="F15" r:id="rId12" display="mailto:sarah.taylor@example.com" xr:uid="{5CFDE6E9-D087-4E1D-8BA1-24C52B201C38}"/>
-    <hyperlink ref="F16" r:id="rId13" display="mailto:john.parker@example.com" xr:uid="{C8F5619E-E92F-4E79-A833-38F9B4BEEF58}"/>
-    <hyperlink ref="F17" r:id="rId14" display="mailto:robert.wilson@example.com" xr:uid="{75FE90AA-72BB-4B81-A820-12FEC320BF5A}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{E556A35B-1BBA-4B19-A0CA-F6385D9E9581}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{9DFE164D-E2A8-4667-9D6B-8F61C02A77AF}"/>
+    <hyperlink ref="F6" r:id="rId3" display="mailto:adam@example.com" xr:uid="{6A4AF44C-6C03-4BD4-B4D2-F2A8A366E654}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{F0483DD7-F3D2-461E-B495-C03875C8D962}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{8721B45D-11B3-4BFD-AFC8-EBEEAEACDA5D}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{0ACC85B6-6103-4AF5-9E36-6AD2972C63AB}"/>
+    <hyperlink ref="F11" r:id="rId7" display="mailto:alex@example.com" xr:uid="{1FCC9A60-CF5F-4058-9BF2-182F9145EA22}"/>
+    <hyperlink ref="F13" r:id="rId8" display="mailto:jennifer@example.com" xr:uid="{F51E6647-6FC6-40FB-BA5C-FC1428669E58}"/>
+    <hyperlink ref="F14" r:id="rId9" display="mailto:alex.green@example.com" xr:uid="{9EDBBE42-7C14-4EA9-A701-5E09B00666AE}"/>
+    <hyperlink ref="F15" r:id="rId10" display="mailto:sarah.taylor@example.com" xr:uid="{5CFDE6E9-D087-4E1D-8BA1-24C52B201C38}"/>
+    <hyperlink ref="F16" r:id="rId11" display="mailto:john.parker@example.com" xr:uid="{C8F5619E-E92F-4E79-A833-38F9B4BEEF58}"/>
+    <hyperlink ref="F17" r:id="rId12" display="mailto:robert.wilson@example.com" xr:uid="{75FE90AA-72BB-4B81-A820-12FEC320BF5A}"/>
+    <hyperlink ref="F3" r:id="rId13" xr:uid="{67032504-2918-45EE-BA50-8C04BED9D910}"/>
+    <hyperlink ref="F2" r:id="rId14" display="mailto:explorer33@packiu.com" xr:uid="{BDFC285A-DDFB-4738-A77A-60F692EB6A41}"/>
+    <hyperlink ref="J4" r:id="rId15" display="StrongP@2ssword1" xr:uid="{7A4F0146-EB93-41A4-A4C2-9790A9636648}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
still added data driver department
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zapta\Automation\Lahebo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A579794D-4190-4B4C-BD1F-C584AE09D2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065A49CC-6926-405F-AA38-570730C5BF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
     <sheet name="SignUp" sheetId="4" r:id="rId2"/>
-    <sheet name="NewUser" sheetId="5" r:id="rId3"/>
-    <sheet name="Client" sheetId="1" r:id="rId4"/>
+    <sheet name="Departments" sheetId="6" r:id="rId3"/>
+    <sheet name="NewUser" sheetId="5" r:id="rId4"/>
+    <sheet name="Client" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="173">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -538,6 +539,15 @@
   </si>
   <si>
     <t>kar8en@example.com</t>
+  </si>
+  <si>
+    <t>DEPARTMENT_NAME</t>
+  </si>
+  <si>
+    <t>DEPARTMENT_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finance </t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1909,6 +1919,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15722E-D9BB-49DC-BBEB-EF0246541F83}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE0024C-58FB-4382-99F9-AF515DDACB52}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1922,7 +1965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>

</xml_diff>

<commit_message>
data provider for department location and job function completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zapta\Automation\Lahebo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065A49CC-6926-405F-AA38-570730C5BF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F1D0AC-BF50-48AD-94B9-795E620D95E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
     <sheet name="SignUp" sheetId="4" r:id="rId2"/>
-    <sheet name="Departments" sheetId="6" r:id="rId3"/>
-    <sheet name="NewUser" sheetId="5" r:id="rId4"/>
-    <sheet name="Client" sheetId="1" r:id="rId5"/>
+    <sheet name="NewUser" sheetId="5" r:id="rId3"/>
+    <sheet name="Departments" sheetId="6" r:id="rId4"/>
+    <sheet name="Locations" sheetId="7" r:id="rId5"/>
+    <sheet name="JobFunction" sheetId="8" r:id="rId6"/>
+    <sheet name="Client" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="183">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -547,14 +549,44 @@
     <t>DEPARTMENT_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">finance </t>
+    <t>design department</t>
+  </si>
+  <si>
+    <t>finance department</t>
+  </si>
+  <si>
+    <t>dev department</t>
+  </si>
+  <si>
+    <t>LOCATION_NAME</t>
+  </si>
+  <si>
+    <t>JOB_FUNCTION_NAME</t>
+  </si>
+  <si>
+    <t>hiring</t>
+  </si>
+  <si>
+    <t>billing</t>
+  </si>
+  <si>
+    <t>typing</t>
+  </si>
+  <si>
+    <t>lahore</t>
+  </si>
+  <si>
+    <t>karachi</t>
+  </si>
+  <si>
+    <t>islamabad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +705,12 @@
       <color rgb="FF444746"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -701,7 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -744,6 +782,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1919,39 +1960,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15722E-D9BB-49DC-BBEB-EF0246541F83}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE0024C-58FB-4382-99F9-AF515DDACB52}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1965,7 +1973,157 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15722E-D9BB-49DC-BBEB-EF0246541F83}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847EB295-5D21-4EA2-B03A-E6270F1C9AEA}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACC492E-FDC2-44DC-BC83-C936F128AC7E}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>

</xml_diff>